<commit_message>
Bugfixed selection issue in naive_dict
</commit_message>
<xml_diff>
--- a/0_1_Output_Data/4_naive_forecaster_qoq_error_series_20101_20181/AVERAGE_10_6_qoq_errors_first_eval_20101_20181.xlsx
+++ b/0_1_Output_Data/4_naive_forecaster_qoq_error_series_20101_20181/AVERAGE_10_6_qoq_errors_first_eval_20101_20181.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Q0</t>
   </si>
@@ -37,97 +37,49 @@
     <t>Q6</t>
   </si>
   <si>
-    <t>2010-01-01 00:00:00_diff</t>
-  </si>
-  <si>
     <t>2010-04-01 00:00:00_diff</t>
   </si>
   <si>
-    <t>2010-07-01 00:00:00_diff</t>
-  </si>
-  <si>
     <t>2010-10-01 00:00:00_diff</t>
   </si>
   <si>
-    <t>2011-01-01 00:00:00_diff</t>
-  </si>
-  <si>
     <t>2011-04-01 00:00:00_diff</t>
   </si>
   <si>
-    <t>2011-07-01 00:00:00_diff</t>
-  </si>
-  <si>
     <t>2011-10-01 00:00:00_diff</t>
   </si>
   <si>
-    <t>2012-01-01 00:00:00_diff</t>
-  </si>
-  <si>
     <t>2012-04-01 00:00:00_diff</t>
   </si>
   <si>
-    <t>2012-07-01 00:00:00_diff</t>
-  </si>
-  <si>
     <t>2012-10-01 00:00:00_diff</t>
   </si>
   <si>
-    <t>2013-01-01 00:00:00_diff</t>
-  </si>
-  <si>
     <t>2013-04-01 00:00:00_diff</t>
   </si>
   <si>
-    <t>2013-07-01 00:00:00_diff</t>
-  </si>
-  <si>
     <t>2013-10-01 00:00:00_diff</t>
   </si>
   <si>
-    <t>2014-01-01 00:00:00_diff</t>
-  </si>
-  <si>
     <t>2014-04-01 00:00:00_diff</t>
   </si>
   <si>
-    <t>2014-07-01 00:00:00_diff</t>
-  </si>
-  <si>
     <t>2014-10-01 00:00:00_diff</t>
   </si>
   <si>
-    <t>2015-01-01 00:00:00_diff</t>
-  </si>
-  <si>
     <t>2015-04-01 00:00:00_diff</t>
   </si>
   <si>
-    <t>2015-07-01 00:00:00_diff</t>
-  </si>
-  <si>
     <t>2015-10-01 00:00:00_diff</t>
   </si>
   <si>
-    <t>2016-01-01 00:00:00_diff</t>
-  </si>
-  <si>
     <t>2016-04-01 00:00:00_diff</t>
   </si>
   <si>
-    <t>2016-07-01 00:00:00_diff</t>
-  </si>
-  <si>
     <t>2016-10-01 00:00:00_diff</t>
   </si>
   <si>
-    <t>2017-01-01 00:00:00_diff</t>
-  </si>
-  <si>
     <t>2017-04-01 00:00:00_diff</t>
-  </si>
-  <si>
-    <t>2017-07-01 00:00:00_diff</t>
   </si>
   <si>
     <t>2017-10-01 00:00:00_diff</t>
@@ -491,7 +443,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -525,25 +477,25 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>-0.4753377773606906</v>
+        <v>-2.542893978309402</v>
       </c>
       <c r="C2">
-        <v>-2.496078019137359</v>
+        <v>-1.058818344549643</v>
       </c>
       <c r="D2">
-        <v>-1.0120023853776</v>
+        <v>-0.7255992615881137</v>
       </c>
       <c r="E2">
-        <v>-0.6787833024160707</v>
+        <v>-1.859984444184283</v>
       </c>
       <c r="F2">
-        <v>-1.81316848501224</v>
+        <v>-0.4800244837065165</v>
       </c>
       <c r="G2">
-        <v>-0.4332085245344734</v>
+        <v>-0.8638202886166834</v>
       </c>
       <c r="H2">
-        <v>-0.8170043294446403</v>
+        <v>-0.1789343978423749</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -551,25 +503,25 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>-2.542893978309402</v>
+        <v>-0.5351204465965399</v>
       </c>
       <c r="C3">
-        <v>-1.058818344549643</v>
+        <v>-1.66950562919271</v>
       </c>
       <c r="D3">
-        <v>-0.7255992615881137</v>
+        <v>-0.2895456687149427</v>
       </c>
       <c r="E3">
-        <v>-1.859984444184283</v>
+        <v>-0.6733414736251095</v>
       </c>
       <c r="F3">
-        <v>-0.4800244837065165</v>
+        <v>0.0115444171491989</v>
       </c>
       <c r="G3">
-        <v>-0.8638202886166834</v>
+        <v>-0.6804809672324722</v>
       </c>
       <c r="H3">
-        <v>-0.1789343978423749</v>
+        <v>-0.4410326232298434</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -577,25 +529,25 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>-0.8243033945289489</v>
+        <v>0.01136921538350649</v>
       </c>
       <c r="C4">
-        <v>-0.4910843115674192</v>
+        <v>-0.3724265895266604</v>
       </c>
       <c r="D4">
-        <v>-1.625469494163589</v>
+        <v>0.3124593012476481</v>
       </c>
       <c r="E4">
-        <v>-0.245509533685822</v>
+        <v>-0.3795660831340231</v>
       </c>
       <c r="F4">
-        <v>-0.6293053385959889</v>
+        <v>-0.1401177391313942</v>
       </c>
       <c r="G4">
-        <v>0.05558055217831959</v>
+        <v>-0.1033897623722235</v>
       </c>
       <c r="H4">
-        <v>-0.6364448322033516</v>
+        <v>0.723104312015092</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -603,25 +555,25 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>-0.5351204465965399</v>
+        <v>0.9526635850093691</v>
       </c>
       <c r="C5">
-        <v>-1.66950562919271</v>
+        <v>0.2606382006276979</v>
       </c>
       <c r="D5">
-        <v>-0.2895456687149427</v>
+        <v>0.5000865446303268</v>
       </c>
       <c r="E5">
-        <v>-0.6733414736251095</v>
+        <v>0.5368145213894975</v>
       </c>
       <c r="F5">
-        <v>0.0115444171491989</v>
+        <v>1.363308595776813</v>
       </c>
       <c r="G5">
-        <v>-0.6804809672324722</v>
+        <v>0.7075103856552477</v>
       </c>
       <c r="H5">
-        <v>-0.4410326232298434</v>
+        <v>0.0493601459296269</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -629,25 +581,25 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>-1.564154328600046</v>
+        <v>0.4274989419678774</v>
       </c>
       <c r="C6">
-        <v>-0.1841943681222787</v>
+        <v>0.4642269187270481</v>
       </c>
       <c r="D6">
-        <v>-0.5679901730324456</v>
+        <v>1.290720993114364</v>
       </c>
       <c r="E6">
-        <v>0.1168957177418629</v>
+        <v>0.6349227829927984</v>
       </c>
       <c r="F6">
-        <v>-0.5751296666398082</v>
+        <v>-0.02322745673282245</v>
       </c>
       <c r="G6">
-        <v>-0.3356813226371794</v>
+        <v>0.3758874911189606</v>
       </c>
       <c r="H6">
-        <v>-0.2989533458780087</v>
+        <v>0.3144509489973832</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -655,25 +607,25 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.01136921538350649</v>
+        <v>1.235029948750828</v>
       </c>
       <c r="C7">
-        <v>-0.3724265895266604</v>
+        <v>0.5792317386292632</v>
       </c>
       <c r="D7">
-        <v>0.3124593012476481</v>
+        <v>-0.07891850109635756</v>
       </c>
       <c r="E7">
-        <v>-0.3795660831340231</v>
+        <v>0.3201964467554255</v>
       </c>
       <c r="F7">
-        <v>-0.1401177391313942</v>
+        <v>0.2587599046338481</v>
       </c>
       <c r="G7">
-        <v>-0.1033897623722235</v>
+        <v>-0.1754060304832554</v>
       </c>
       <c r="H7">
-        <v>0.723104312015092</v>
+        <v>0.8033953615958215</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -681,25 +633,25 @@
         <v>13</v>
       </c>
       <c r="B8">
-        <v>-0.1989446793676382</v>
+        <v>-0.4329776612703231</v>
       </c>
       <c r="C8">
-        <v>0.4859412114066703</v>
+        <v>-0.03386271341853997</v>
       </c>
       <c r="D8">
-        <v>-0.2060841729750008</v>
+        <v>-0.09529925554011737</v>
       </c>
       <c r="E8">
-        <v>0.03336417102762801</v>
+        <v>-0.529465190657221</v>
       </c>
       <c r="F8">
-        <v>0.07009214778679873</v>
+        <v>0.449336201421856</v>
       </c>
       <c r="G8">
-        <v>0.8965862221741142</v>
+        <v>0.2222202969739298</v>
       </c>
       <c r="H8">
-        <v>0.240788012052549</v>
+        <v>-0.4112394324521587</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -707,25 +659,25 @@
         <v>14</v>
       </c>
       <c r="B9">
-        <v>0.9526635850093691</v>
+        <v>-0.1856174723396913</v>
       </c>
       <c r="C9">
-        <v>0.2606382006276979</v>
+        <v>-0.6197834074567948</v>
       </c>
       <c r="D9">
-        <v>0.5000865446303268</v>
+        <v>0.3590179846222821</v>
       </c>
       <c r="E9">
-        <v>0.5368145213894975</v>
+        <v>0.1319020801743559</v>
       </c>
       <c r="F9">
-        <v>1.363308595776813</v>
+        <v>-0.5015576492517326</v>
       </c>
       <c r="G9">
-        <v>0.7075103856552477</v>
+        <v>-0.07416069059612829</v>
       </c>
       <c r="H9">
-        <v>0.0493601459296269</v>
+        <v>-0.2404976452842752</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -733,25 +685,25 @@
         <v>15</v>
       </c>
       <c r="B10">
-        <v>0.2183276878862375</v>
+        <v>0.4273407187267424</v>
       </c>
       <c r="C10">
-        <v>0.4577760318888663</v>
+        <v>0.2002248142788162</v>
       </c>
       <c r="D10">
-        <v>0.494504008648037</v>
+        <v>-0.4332349151472724</v>
       </c>
       <c r="E10">
-        <v>1.320998083035352</v>
+        <v>-0.005837956491668017</v>
       </c>
       <c r="F10">
-        <v>0.6651998729137872</v>
+        <v>-0.1721749111798149</v>
       </c>
       <c r="G10">
-        <v>0.007049633188166426</v>
+        <v>-0.0494638947389891</v>
       </c>
       <c r="H10">
-        <v>0.4061645810399495</v>
+        <v>-0.002230158183848807</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -759,25 +711,25 @@
         <v>16</v>
       </c>
       <c r="B11">
-        <v>0.4274989419678774</v>
+        <v>-0.5318964931771777</v>
       </c>
       <c r="C11">
-        <v>0.4642269187270481</v>
+        <v>-0.1044995345215733</v>
       </c>
       <c r="D11">
-        <v>1.290720993114364</v>
+        <v>-0.2708364892097202</v>
       </c>
       <c r="E11">
-        <v>0.6349227829927984</v>
+        <v>-0.1481254727688944</v>
       </c>
       <c r="F11">
-        <v>-0.02322745673282245</v>
+        <v>-0.1008917362137541</v>
       </c>
       <c r="G11">
-        <v>0.3758874911189606</v>
+        <v>-0.4975104677362057</v>
       </c>
       <c r="H11">
-        <v>0.3144509489973832</v>
+        <v>-0.2434584326124856</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -785,25 +737,25 @@
         <v>17</v>
       </c>
       <c r="B12">
-        <v>0.451611734653072</v>
+        <v>-0.1938269109680474</v>
       </c>
       <c r="C12">
-        <v>1.278105809040388</v>
+        <v>-0.07111589452722158</v>
       </c>
       <c r="D12">
-        <v>0.6223075989188223</v>
+        <v>-0.02388215797208129</v>
       </c>
       <c r="E12">
-        <v>-0.03584264080679855</v>
+        <v>-0.4205008894945329</v>
       </c>
       <c r="F12">
-        <v>0.3632723070449845</v>
+        <v>-0.1664488543708128</v>
       </c>
       <c r="G12">
-        <v>0.3018357649234071</v>
+        <v>0.0536755355027598</v>
       </c>
       <c r="H12">
-        <v>-0.1323301701936964</v>
+        <v>-0.1821129130839084</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -811,25 +763,25 @@
         <v>18</v>
       </c>
       <c r="B13">
-        <v>1.235029948750828</v>
+        <v>0.1476338940440795</v>
       </c>
       <c r="C13">
-        <v>0.5792317386292632</v>
+        <v>-0.2489848374783721</v>
       </c>
       <c r="D13">
-        <v>-0.07891850109635756</v>
+        <v>0.005067197645347965</v>
       </c>
       <c r="E13">
-        <v>0.3201964467554255</v>
+        <v>0.2251915875189206</v>
       </c>
       <c r="F13">
-        <v>0.2587599046338481</v>
+        <v>-0.0105968610677476</v>
       </c>
       <c r="G13">
-        <v>-0.1754060304832554</v>
+        <v>-0.1895696185385323</v>
       </c>
       <c r="H13">
-        <v>0.8033953615958215</v>
+        <v>-0.2001301487978533</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -837,25 +789,25 @@
         <v>19</v>
       </c>
       <c r="B14">
-        <v>0.299808989306214</v>
+        <v>-0.0323979044984018</v>
       </c>
       <c r="C14">
-        <v>-0.3583412504194069</v>
+        <v>0.1877264853751708</v>
       </c>
       <c r="D14">
-        <v>0.04077369743237619</v>
+        <v>-0.04806196321149736</v>
       </c>
       <c r="E14">
-        <v>-0.02066284468920121</v>
+        <v>-0.2270347206822821</v>
       </c>
       <c r="F14">
-        <v>-0.4548287798063048</v>
+        <v>-0.2375952509416031</v>
       </c>
       <c r="G14">
-        <v>0.5239726122727721</v>
+        <v>-0.4453143610997332</v>
       </c>
       <c r="H14">
-        <v>0.296856707824846</v>
+        <v>-0.2281054616248284</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -863,25 +815,25 @@
         <v>20</v>
       </c>
       <c r="B15">
-        <v>-0.4329776612703231</v>
+        <v>-0.06996447561954</v>
       </c>
       <c r="C15">
-        <v>-0.03386271341853997</v>
+        <v>-0.2489372330903247</v>
       </c>
       <c r="D15">
-        <v>-0.09529925554011737</v>
+        <v>-0.2594977633496457</v>
       </c>
       <c r="E15">
-        <v>-0.529465190657221</v>
+        <v>-0.4672168735077758</v>
       </c>
       <c r="F15">
-        <v>0.449336201421856</v>
+        <v>-0.2500079740328711</v>
       </c>
       <c r="G15">
-        <v>0.2222202969739298</v>
+        <v>0.05967819522519041</v>
       </c>
       <c r="H15">
-        <v>-0.4112394324521587</v>
+        <v>-0.09462593860681362</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -889,25 +841,25 @@
         <v>21</v>
       </c>
       <c r="B16">
-        <v>-0.00299340778301399</v>
+        <v>-0.1713918715036764</v>
       </c>
       <c r="C16">
-        <v>-0.06442994990459139</v>
+        <v>-0.3791109816618064</v>
       </c>
       <c r="D16">
-        <v>-0.4985958850216949</v>
+        <v>-0.1619020821869017</v>
       </c>
       <c r="E16">
-        <v>0.480205507057382</v>
+        <v>0.1477840870711598</v>
       </c>
       <c r="F16">
-        <v>0.2530896026094558</v>
+        <v>-0.006520046760844223</v>
       </c>
       <c r="G16">
-        <v>-0.3803701268166327</v>
+        <v>0.643906374458339</v>
       </c>
       <c r="H16">
-        <v>0.04702683183897161</v>
+        <v>0.4277413258401298</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -915,25 +867,25 @@
         <v>22</v>
       </c>
       <c r="B17">
-        <v>-0.1856174723396913</v>
+        <v>-0.06818896562035748</v>
       </c>
       <c r="C17">
-        <v>-0.6197834074567948</v>
+        <v>0.241497203637704</v>
       </c>
       <c r="D17">
-        <v>0.3590179846222821</v>
+        <v>0.08719306980569996</v>
       </c>
       <c r="E17">
-        <v>0.1319020801743559</v>
+        <v>0.7376194910248832</v>
       </c>
       <c r="F17">
-        <v>-0.5015576492517326</v>
+        <v>0.521454442406674</v>
       </c>
       <c r="G17">
-        <v>-0.07416069059612829</v>
+        <v>0.1144253133717177</v>
       </c>
       <c r="H17">
-        <v>-0.2404976452842752</v>
+        <v>0.6134675305491375</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -941,440 +893,24 @@
         <v>23</v>
       </c>
       <c r="B18">
-        <v>-0.5905101764174595</v>
+        <v>0.2497007499081394</v>
       </c>
       <c r="C18">
-        <v>0.3882912156616174</v>
+        <v>0.09539661607613537</v>
       </c>
       <c r="D18">
-        <v>0.1611753112136912</v>
+        <v>0.7458230372953185</v>
       </c>
       <c r="E18">
-        <v>-0.4722844182123973</v>
+        <v>0.5296579886771094</v>
       </c>
       <c r="F18">
-        <v>-0.04488745955679299</v>
+        <v>0.1226288596421531</v>
       </c>
       <c r="G18">
-        <v>-0.2112244142449399</v>
+        <v>0.6216710768195729</v>
       </c>
       <c r="H18">
-        <v>-0.08851339780411407</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19">
-        <v>0.4273407187267424</v>
-      </c>
-      <c r="C19">
-        <v>0.2002248142788162</v>
-      </c>
-      <c r="D19">
-        <v>-0.4332349151472724</v>
-      </c>
-      <c r="E19">
-        <v>-0.005837956491668017</v>
-      </c>
-      <c r="F19">
-        <v>-0.1721749111798149</v>
-      </c>
-      <c r="G19">
-        <v>-0.0494638947389891</v>
-      </c>
-      <c r="H19">
-        <v>-0.002230158183848807</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20">
-        <v>0.1086983409703039</v>
-      </c>
-      <c r="C20">
-        <v>-0.5247613884557847</v>
-      </c>
-      <c r="D20">
-        <v>-0.09736442980018029</v>
-      </c>
-      <c r="E20">
-        <v>-0.2637013844883272</v>
-      </c>
-      <c r="F20">
-        <v>-0.1409903680475014</v>
-      </c>
-      <c r="G20">
-        <v>-0.09375663149236108</v>
-      </c>
-      <c r="H20">
-        <v>-0.4903753630148127</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21">
-        <v>-0.5318964931771777</v>
-      </c>
-      <c r="C21">
-        <v>-0.1044995345215733</v>
-      </c>
-      <c r="D21">
-        <v>-0.2708364892097202</v>
-      </c>
-      <c r="E21">
-        <v>-0.1481254727688944</v>
-      </c>
-      <c r="F21">
-        <v>-0.1008917362137541</v>
-      </c>
-      <c r="G21">
-        <v>-0.4975104677362057</v>
-      </c>
-      <c r="H21">
-        <v>-0.2434584326124856</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22">
-        <v>-0.04607696087735</v>
-      </c>
-      <c r="C22">
-        <v>-0.2124139155654969</v>
-      </c>
-      <c r="D22">
-        <v>-0.08970289912467108</v>
-      </c>
-      <c r="E22">
-        <v>-0.04246916256953079</v>
-      </c>
-      <c r="F22">
-        <v>-0.4390878940919825</v>
-      </c>
-      <c r="G22">
-        <v>-0.1850358589682623</v>
-      </c>
-      <c r="H22">
-        <v>0.03508853090531031</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23">
-        <v>-0.1938269109680474</v>
-      </c>
-      <c r="C23">
-        <v>-0.07111589452722158</v>
-      </c>
-      <c r="D23">
-        <v>-0.02388215797208129</v>
-      </c>
-      <c r="E23">
-        <v>-0.4205008894945329</v>
-      </c>
-      <c r="F23">
-        <v>-0.1664488543708128</v>
-      </c>
-      <c r="G23">
-        <v>0.0536755355027598</v>
-      </c>
-      <c r="H23">
-        <v>-0.1821129130839084</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24">
-        <v>0.04184555234415971</v>
-      </c>
-      <c r="C24">
-        <v>0.0890792888993</v>
-      </c>
-      <c r="D24">
-        <v>-0.3075394426231516</v>
-      </c>
-      <c r="E24">
-        <v>-0.05348740749943154</v>
-      </c>
-      <c r="F24">
-        <v>0.1666369823741411</v>
-      </c>
-      <c r="G24">
-        <v>-0.0691514662125271</v>
-      </c>
-      <c r="H24">
-        <v>-0.2481242236833118</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25">
-        <v>0.1476338940440795</v>
-      </c>
-      <c r="C25">
-        <v>-0.2489848374783721</v>
-      </c>
-      <c r="D25">
-        <v>0.005067197645347965</v>
-      </c>
-      <c r="E25">
-        <v>0.2251915875189206</v>
-      </c>
-      <c r="F25">
-        <v>-0.0105968610677476</v>
-      </c>
-      <c r="G25">
-        <v>-0.1895696185385323</v>
-      </c>
-      <c r="H25">
-        <v>-0.2001301487978533</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26">
-        <v>-0.31566407673435</v>
-      </c>
-      <c r="C26">
-        <v>-0.06161204161062994</v>
-      </c>
-      <c r="D26">
-        <v>0.1585123482629427</v>
-      </c>
-      <c r="E26">
-        <v>-0.07727610032372551</v>
-      </c>
-      <c r="F26">
-        <v>-0.2562488577945102</v>
-      </c>
-      <c r="G26">
-        <v>-0.2668093880538313</v>
-      </c>
-      <c r="H26">
-        <v>-0.4745284982119613</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27">
-        <v>-0.0323979044984018</v>
-      </c>
-      <c r="C27">
-        <v>0.1877264853751708</v>
-      </c>
-      <c r="D27">
-        <v>-0.04806196321149736</v>
-      </c>
-      <c r="E27">
-        <v>-0.2270347206822821</v>
-      </c>
-      <c r="F27">
-        <v>-0.2375952509416031</v>
-      </c>
-      <c r="G27">
-        <v>-0.4453143610997332</v>
-      </c>
-      <c r="H27">
-        <v>-0.2281054616248284</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B28">
-        <v>0.2063695661061287</v>
-      </c>
-      <c r="C28">
-        <v>-0.02941888248053948</v>
-      </c>
-      <c r="D28">
-        <v>-0.2083916399513242</v>
-      </c>
-      <c r="E28">
-        <v>-0.2189521702106452</v>
-      </c>
-      <c r="F28">
-        <v>-0.4266712803687753</v>
-      </c>
-      <c r="G28">
-        <v>-0.2094623808938705</v>
-      </c>
-      <c r="H28">
-        <v>0.1002237883641909</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B29">
-        <v>-0.06996447561954</v>
-      </c>
-      <c r="C29">
-        <v>-0.2489372330903247</v>
-      </c>
-      <c r="D29">
-        <v>-0.2594977633496457</v>
-      </c>
-      <c r="E29">
-        <v>-0.4672168735077758</v>
-      </c>
-      <c r="F29">
-        <v>-0.2500079740328711</v>
-      </c>
-      <c r="G29">
-        <v>0.05967819522519041</v>
-      </c>
-      <c r="H29">
-        <v>-0.09462593860681362</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B30">
-        <v>-0.1949601066790565</v>
-      </c>
-      <c r="C30">
-        <v>-0.2055206369383775</v>
-      </c>
-      <c r="D30">
-        <v>-0.4132397470965076</v>
-      </c>
-      <c r="E30">
-        <v>-0.1960308476216028</v>
-      </c>
-      <c r="F30">
-        <v>0.1136553216364586</v>
-      </c>
-      <c r="G30">
-        <v>-0.04064881219554539</v>
-      </c>
-      <c r="H30">
-        <v>0.6097776090236378</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B31">
-        <v>-0.1713918715036764</v>
-      </c>
-      <c r="C31">
-        <v>-0.3791109816618064</v>
-      </c>
-      <c r="D31">
-        <v>-0.1619020821869017</v>
-      </c>
-      <c r="E31">
-        <v>0.1477840870711598</v>
-      </c>
-      <c r="F31">
-        <v>-0.006520046760844223</v>
-      </c>
-      <c r="G31">
-        <v>0.643906374458339</v>
-      </c>
-      <c r="H31">
-        <v>0.4277413258401298</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32">
-        <v>-0.3763423975016759</v>
-      </c>
-      <c r="C32">
-        <v>-0.1591334980267711</v>
-      </c>
-      <c r="D32">
-        <v>0.1505526712312903</v>
-      </c>
-      <c r="E32">
-        <v>-0.003751462600713684</v>
-      </c>
-      <c r="F32">
-        <v>0.6466749586184695</v>
-      </c>
-      <c r="G32">
-        <v>0.4305099100002604</v>
-      </c>
-      <c r="H32">
-        <v>0.02348078096530404</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B33">
-        <v>-0.06818896562035748</v>
-      </c>
-      <c r="C33">
-        <v>0.241497203637704</v>
-      </c>
-      <c r="D33">
-        <v>0.08719306980569996</v>
-      </c>
-      <c r="E33">
-        <v>0.7376194910248832</v>
-      </c>
-      <c r="F33">
-        <v>0.521454442406674</v>
-      </c>
-      <c r="G33">
-        <v>0.1144253133717177</v>
-      </c>
-      <c r="H33">
-        <v>0.6134675305491375</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B34">
-        <v>0.2497007499081394</v>
-      </c>
-      <c r="C34">
-        <v>0.09539661607613537</v>
-      </c>
-      <c r="D34">
-        <v>0.7458230372953185</v>
-      </c>
-      <c r="E34">
-        <v>0.5296579886771094</v>
-      </c>
-      <c r="F34">
-        <v>0.1226288596421531</v>
-      </c>
-      <c r="G34">
-        <v>0.6216710768195729</v>
-      </c>
-      <c r="H34">
         <v>0.4628221636640603</v>
       </c>
     </row>

</xml_diff>